<commit_message>
final step of my project
</commit_message>
<xml_diff>
--- a/Task/src/test/resources/places.xlsx
+++ b/Task/src/test/resources/places.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkPlace\Tasks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mburk/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B352C4-6044-F547-BCDB-085E50588ABD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="9540" yWindow="3440" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>lat</t>
   </si>
@@ -42,30 +43,12 @@
   </si>
   <si>
     <t>Ivano-Frankivsk</t>
-  </si>
-  <si>
-    <t>50.450100</t>
-  </si>
-  <si>
-    <t>30.523400</t>
-  </si>
-  <si>
-    <t>49.839683</t>
-  </si>
-  <si>
-    <t>24.029717</t>
-  </si>
-  <si>
-    <t>48.922633</t>
-  </si>
-  <si>
-    <t>24.711117</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -387,21 +370,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -412,37 +395,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
+      <c r="B2">
+        <v>50.447730999999997</v>
+      </c>
+      <c r="C2">
+        <v>30.542721</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
+      <c r="B3">
+        <v>49.839683999999998</v>
+      </c>
+      <c r="C3">
+        <v>24.029716000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
+      <c r="B4">
+        <v>48.922634000000002</v>
+      </c>
+      <c r="C4">
+        <v>24.711117000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>